<commit_message>
Garbage Cleaning. Added .icc profiles, Matlab analysis scripts and csv files containing raw and cleaned data.
</commit_message>
<xml_diff>
--- a/Documents/Questoes e Respostas.xlsx
+++ b/Documents/Questoes e Respostas.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="60">
   <si>
     <t>Questão</t>
   </si>
@@ -190,6 +190,21 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Perguntas com cores dadas iguais:</t>
+  </si>
+  <si>
+    <t>#3 + #12</t>
+  </si>
+  <si>
+    <t>#6 + #11</t>
+  </si>
+  <si>
+    <t>#9 + #15</t>
+  </si>
+  <si>
+    <t>#10 + #13</t>
   </si>
 </sst>
 </file>
@@ -481,7 +496,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -600,6 +615,36 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -624,12 +669,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -676,18 +715,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -985,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1000,30 +1027,30 @@
     <col min="10" max="10" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:13" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="66"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="66" t="s">
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="67"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="45"/>
       <c r="J2" s="17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1045,15 +1072,18 @@
       <c r="G3" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="68" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="69"/>
+      <c r="H3" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="47"/>
       <c r="J3" s="7">
         <v>138</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1082,8 +1112,14 @@
       <c r="J4" s="7">
         <v>139</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L4" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1112,8 +1148,14 @@
       <c r="J5" s="7">
         <v>133</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L5" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1142,8 +1184,14 @@
       <c r="J6" s="7">
         <v>132</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L6" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="M6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1172,8 +1220,14 @@
       <c r="J7" s="7">
         <v>138</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L7" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="M7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1203,7 +1257,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1233,7 +1287,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1263,7 +1317,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1293,7 +1347,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1323,7 +1377,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1353,7 +1407,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1383,7 +1437,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -1413,7 +1467,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1555,10 +1609,10 @@
       <c r="G20" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H20" s="50" t="s">
+      <c r="H20" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="I20" s="51"/>
+      <c r="I20" s="59"/>
       <c r="J20" s="7">
         <v>140</v>
       </c>
@@ -1585,10 +1639,10 @@
       <c r="G21" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H21" s="52" t="s">
+      <c r="H21" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="I21" s="53"/>
+      <c r="I21" s="61"/>
       <c r="J21" s="7">
         <v>139</v>
       </c>
@@ -1615,10 +1669,10 @@
       <c r="G22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H22" s="54" t="s">
+      <c r="H22" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="I22" s="55"/>
+      <c r="I22" s="63"/>
       <c r="J22" s="7">
         <v>135</v>
       </c>
@@ -1677,10 +1731,10 @@
       <c r="G24" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H24" s="64" t="s">
+      <c r="H24" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="I24" s="65"/>
+      <c r="I24" s="73"/>
       <c r="J24" s="7">
         <v>136</v>
       </c>
@@ -1707,10 +1761,10 @@
       <c r="G25" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H25" s="62" t="s">
+      <c r="H25" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="I25" s="63"/>
+      <c r="I25" s="71"/>
       <c r="J25" s="7">
         <v>139</v>
       </c>
@@ -1737,10 +1791,10 @@
       <c r="G26" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H26" s="60" t="s">
+      <c r="H26" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="I26" s="61"/>
+      <c r="I26" s="69"/>
       <c r="J26" s="7">
         <v>139</v>
       </c>
@@ -1767,10 +1821,10 @@
       <c r="G27" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H27" s="58" t="s">
+      <c r="H27" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="I27" s="59"/>
+      <c r="I27" s="67"/>
       <c r="J27" s="7">
         <v>143</v>
       </c>
@@ -1797,10 +1851,10 @@
       <c r="G28" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H28" s="56" t="s">
+      <c r="H28" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="I28" s="57"/>
+      <c r="I28" s="65"/>
       <c r="J28" s="7">
         <v>141</v>
       </c>
@@ -1859,10 +1913,10 @@
       <c r="G30" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H30" s="46" t="s">
+      <c r="H30" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="I30" s="47"/>
+      <c r="I30" s="57"/>
       <c r="J30" s="7">
         <v>146</v>
       </c>
@@ -1889,10 +1943,10 @@
       <c r="G31" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H31" s="44" t="s">
+      <c r="H31" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="I31" s="45"/>
+      <c r="I31" s="55"/>
       <c r="J31" s="7">
         <v>137</v>
       </c>
@@ -1919,10 +1973,10 @@
       <c r="G32" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H32" s="42" t="s">
+      <c r="H32" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="I32" s="43"/>
+      <c r="I32" s="53"/>
       <c r="J32" s="7">
         <v>135</v>
       </c>
@@ -1981,33 +2035,16 @@
       <c r="G34" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="H34" s="40" t="s">
+      <c r="H34" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="I34" s="41"/>
+      <c r="I34" s="51"/>
       <c r="J34" s="15">
         <v>138</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
     <mergeCell ref="H34:I34"/>
     <mergeCell ref="H32:I32"/>
     <mergeCell ref="H31:I31"/>
@@ -2022,6 +2059,23 @@
     <mergeCell ref="H26:I26"/>
     <mergeCell ref="H25:I25"/>
     <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cleaning and Processing DONE. NEXT: Results.
</commit_message>
<xml_diff>
--- a/Documents/Questoes e Respostas.xlsx
+++ b/Documents/Questoes e Respostas.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Perguntas" sheetId="1" r:id="rId1"/>
-    <sheet name="Conclusões" sheetId="2" r:id="rId2"/>
+    <sheet name="Contagem" sheetId="3" r:id="rId2"/>
+    <sheet name="Conclusões" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="81">
   <si>
     <t>Questão</t>
   </si>
@@ -205,6 +206,69 @@
   </si>
   <si>
     <t>#10 + #13</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Given Colors</t>
+  </si>
+  <si>
+    <t>Expected Results</t>
+  </si>
+  <si>
+    <t>Color C1</t>
+  </si>
+  <si>
+    <t>Color C2</t>
+  </si>
+  <si>
+    <t>Color C3</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Lab</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>Age &lt; 20</t>
+  </si>
+  <si>
+    <t>20 &lt; Age &lt; 29</t>
+  </si>
+  <si>
+    <t>30 &lt; Age &lt; 39</t>
+  </si>
+  <si>
+    <t>40 &lt; Age &lt; 49</t>
+  </si>
+  <si>
+    <t>50 &lt; Age &lt; 59</t>
+  </si>
+  <si>
+    <t>Age &gt; 60</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Counting</t>
   </si>
 </sst>
 </file>
@@ -335,7 +399,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -488,6 +552,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -496,7 +573,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -627,6 +704,135 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -639,82 +845,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1014,7 +1155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
@@ -1035,17 +1176,17 @@
       <c r="B2" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="44" t="s">
+      <c r="D2" s="87"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="45"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="88"/>
       <c r="J2" s="17" t="s">
         <v>36</v>
       </c>
@@ -1072,10 +1213,10 @@
       <c r="G3" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="46" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="47"/>
+      <c r="H3" s="89" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="90"/>
       <c r="J3" s="7">
         <v>138</v>
       </c>
@@ -1105,10 +1246,10 @@
       <c r="G4" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="I4" s="49"/>
+      <c r="H4" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="70"/>
       <c r="J4" s="7">
         <v>139</v>
       </c>
@@ -1141,10 +1282,10 @@
       <c r="G5" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="I5" s="49"/>
+      <c r="H5" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="70"/>
       <c r="J5" s="7">
         <v>133</v>
       </c>
@@ -1177,10 +1318,10 @@
       <c r="G6" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H6" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="I6" s="49"/>
+      <c r="H6" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" s="70"/>
       <c r="J6" s="7">
         <v>132</v>
       </c>
@@ -1213,10 +1354,10 @@
       <c r="G7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="I7" s="49"/>
+      <c r="H7" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="70"/>
       <c r="J7" s="7">
         <v>138</v>
       </c>
@@ -1249,10 +1390,10 @@
       <c r="G8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="I8" s="49"/>
+      <c r="H8" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="70"/>
       <c r="J8" s="7">
         <v>128</v>
       </c>
@@ -1279,10 +1420,10 @@
       <c r="G9" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H9" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="I9" s="49"/>
+      <c r="H9" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="70"/>
       <c r="J9" s="7">
         <v>140</v>
       </c>
@@ -1309,10 +1450,10 @@
       <c r="G10" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H10" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="I10" s="49"/>
+      <c r="H10" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="70"/>
       <c r="J10" s="7">
         <v>129</v>
       </c>
@@ -1339,10 +1480,10 @@
       <c r="G11" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="I11" s="49"/>
+      <c r="H11" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" s="70"/>
       <c r="J11" s="7">
         <v>136</v>
       </c>
@@ -1369,10 +1510,10 @@
       <c r="G12" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H12" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="I12" s="49"/>
+      <c r="H12" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="70"/>
       <c r="J12" s="7">
         <v>136</v>
       </c>
@@ -1399,10 +1540,10 @@
       <c r="G13" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H13" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="I13" s="49"/>
+      <c r="H13" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="70"/>
       <c r="J13" s="7">
         <v>130</v>
       </c>
@@ -1429,10 +1570,10 @@
       <c r="G14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H14" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="I14" s="49"/>
+      <c r="H14" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14" s="70"/>
       <c r="J14" s="7">
         <v>122</v>
       </c>
@@ -1459,10 +1600,10 @@
       <c r="G15" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H15" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="I15" s="49"/>
+      <c r="H15" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" s="70"/>
       <c r="J15" s="7">
         <v>135</v>
       </c>
@@ -1489,10 +1630,10 @@
       <c r="G16" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H16" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="I16" s="49"/>
+      <c r="H16" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" s="70"/>
       <c r="J16" s="7">
         <v>133</v>
       </c>
@@ -1519,10 +1660,10 @@
       <c r="G17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H17" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="I17" s="49"/>
+      <c r="H17" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17" s="70"/>
       <c r="J17" s="7">
         <v>135</v>
       </c>
@@ -1549,10 +1690,10 @@
       <c r="G18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H18" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="I18" s="49"/>
+      <c r="H18" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I18" s="70"/>
       <c r="J18" s="7">
         <v>140</v>
       </c>
@@ -1579,10 +1720,10 @@
       <c r="G19" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="I19" s="49"/>
+      <c r="H19" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19" s="70"/>
       <c r="J19" s="7">
         <v>130</v>
       </c>
@@ -1609,10 +1750,10 @@
       <c r="G20" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H20" s="58" t="s">
+      <c r="H20" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="I20" s="59"/>
+      <c r="I20" s="72"/>
       <c r="J20" s="7">
         <v>140</v>
       </c>
@@ -1639,10 +1780,10 @@
       <c r="G21" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H21" s="60" t="s">
+      <c r="H21" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="I21" s="61"/>
+      <c r="I21" s="74"/>
       <c r="J21" s="7">
         <v>139</v>
       </c>
@@ -1669,10 +1810,10 @@
       <c r="G22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H22" s="62" t="s">
+      <c r="H22" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="I22" s="63"/>
+      <c r="I22" s="76"/>
       <c r="J22" s="7">
         <v>135</v>
       </c>
@@ -1731,10 +1872,10 @@
       <c r="G24" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H24" s="72" t="s">
+      <c r="H24" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="I24" s="73"/>
+      <c r="I24" s="86"/>
       <c r="J24" s="7">
         <v>136</v>
       </c>
@@ -1761,10 +1902,10 @@
       <c r="G25" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H25" s="70" t="s">
+      <c r="H25" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="I25" s="71"/>
+      <c r="I25" s="84"/>
       <c r="J25" s="7">
         <v>139</v>
       </c>
@@ -1791,10 +1932,10 @@
       <c r="G26" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H26" s="68" t="s">
+      <c r="H26" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="I26" s="69"/>
+      <c r="I26" s="82"/>
       <c r="J26" s="7">
         <v>139</v>
       </c>
@@ -1821,10 +1962,10 @@
       <c r="G27" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H27" s="66" t="s">
+      <c r="H27" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="I27" s="67"/>
+      <c r="I27" s="80"/>
       <c r="J27" s="7">
         <v>143</v>
       </c>
@@ -1851,10 +1992,10 @@
       <c r="G28" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H28" s="64" t="s">
+      <c r="H28" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="I28" s="65"/>
+      <c r="I28" s="78"/>
       <c r="J28" s="7">
         <v>141</v>
       </c>
@@ -1913,10 +2054,10 @@
       <c r="G30" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H30" s="56" t="s">
+      <c r="H30" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="I30" s="57"/>
+      <c r="I30" s="68"/>
       <c r="J30" s="7">
         <v>146</v>
       </c>
@@ -1943,10 +2084,10 @@
       <c r="G31" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H31" s="54" t="s">
+      <c r="H31" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="I31" s="55"/>
+      <c r="I31" s="66"/>
       <c r="J31" s="7">
         <v>137</v>
       </c>
@@ -1973,10 +2114,10 @@
       <c r="G32" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H32" s="52" t="s">
+      <c r="H32" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="I32" s="53"/>
+      <c r="I32" s="64"/>
       <c r="J32" s="7">
         <v>135</v>
       </c>
@@ -2035,16 +2176,33 @@
       <c r="G34" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="H34" s="50" t="s">
+      <c r="H34" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="I34" s="51"/>
+      <c r="I34" s="62"/>
       <c r="J34" s="15">
         <v>138</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
     <mergeCell ref="H34:I34"/>
     <mergeCell ref="H32:I32"/>
     <mergeCell ref="H31:I31"/>
@@ -2059,29 +2217,1246 @@
     <mergeCell ref="H26:I26"/>
     <mergeCell ref="H25:I25"/>
     <mergeCell ref="H24:I24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4:K35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" style="1" customWidth="1"/>
+    <col min="3" max="7" width="9.83203125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="6.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7.1640625" style="1" customWidth="1"/>
+    <col min="11" max="13" width="7.1640625" customWidth="1"/>
+    <col min="14" max="17" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="22" width="7.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:22" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="93" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="93" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="87" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="87"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="87" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="95" t="s">
+        <v>80</v>
+      </c>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="69"/>
+      <c r="P2" s="69"/>
+      <c r="Q2" s="69"/>
+      <c r="R2" s="69"/>
+      <c r="S2" s="69"/>
+      <c r="T2" s="69"/>
+      <c r="U2" s="69"/>
+      <c r="V2" s="69"/>
+    </row>
+    <row r="3" spans="1:22" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="94"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="87" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="88"/>
+      <c r="J3" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="K3" s="92" t="s">
+        <v>68</v>
+      </c>
+      <c r="L3" s="92" t="s">
+        <v>69</v>
+      </c>
+      <c r="M3" s="92" t="s">
+        <v>70</v>
+      </c>
+      <c r="N3" s="92" t="s">
+        <v>71</v>
+      </c>
+      <c r="O3" s="92" t="s">
+        <v>72</v>
+      </c>
+      <c r="P3" s="92" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q3" s="92" t="s">
+        <v>74</v>
+      </c>
+      <c r="R3" s="92" t="s">
+        <v>75</v>
+      </c>
+      <c r="S3" s="92" t="s">
+        <v>76</v>
+      </c>
+      <c r="T3" s="92" t="s">
+        <v>77</v>
+      </c>
+      <c r="U3" s="92" t="s">
+        <v>78</v>
+      </c>
+      <c r="V3" s="92" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="89" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="90"/>
+      <c r="J4" s="45">
+        <v>138</v>
+      </c>
+      <c r="K4">
+        <v>29</v>
+      </c>
+      <c r="L4" s="91"/>
+      <c r="M4" s="91"/>
+    </row>
+    <row r="5" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="70"/>
+      <c r="J5" s="45">
+        <v>139</v>
+      </c>
+      <c r="K5">
+        <v>29</v>
+      </c>
+      <c r="L5" s="92"/>
+      <c r="M5" s="91"/>
+    </row>
+    <row r="6" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" s="70"/>
+      <c r="J6" s="45">
+        <v>133</v>
+      </c>
+      <c r="K6">
+        <v>29</v>
+      </c>
+      <c r="L6" s="92"/>
+      <c r="M6" s="91"/>
+    </row>
+    <row r="7" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="70"/>
+      <c r="J7" s="45">
+        <v>132</v>
+      </c>
+      <c r="K7">
+        <v>29</v>
+      </c>
+      <c r="L7" s="92"/>
+      <c r="M7" s="91"/>
+    </row>
+    <row r="8" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="70"/>
+      <c r="J8" s="45">
+        <v>138</v>
+      </c>
+      <c r="K8">
+        <v>29</v>
+      </c>
+      <c r="L8" s="92"/>
+      <c r="M8" s="91"/>
+    </row>
+    <row r="9" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="70"/>
+      <c r="J9" s="45">
+        <v>128</v>
+      </c>
+      <c r="K9">
+        <v>29</v>
+      </c>
+      <c r="L9" s="91"/>
+      <c r="M9" s="91"/>
+    </row>
+    <row r="10" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="58" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="70"/>
+      <c r="J10" s="45">
+        <v>140</v>
+      </c>
+      <c r="K10">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" s="70"/>
+      <c r="J11" s="45">
+        <v>129</v>
+      </c>
+      <c r="K11">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="70"/>
+      <c r="J12" s="45">
+        <v>136</v>
+      </c>
+      <c r="K12">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="70"/>
+      <c r="J13" s="45">
+        <v>136</v>
+      </c>
+      <c r="K13">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14" s="70"/>
+      <c r="J14" s="45">
+        <v>130</v>
+      </c>
+      <c r="K14">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" s="70"/>
+      <c r="J15" s="45">
+        <v>122</v>
+      </c>
+      <c r="K15">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="H16" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" s="70"/>
+      <c r="J16" s="45">
+        <v>135</v>
+      </c>
+      <c r="K16">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17" s="70"/>
+      <c r="J17" s="45">
+        <v>133</v>
+      </c>
+      <c r="K17">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="H18" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I18" s="70"/>
+      <c r="J18" s="45">
+        <v>135</v>
+      </c>
+      <c r="K18">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="H19" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19" s="70"/>
+      <c r="J19" s="45">
+        <v>140</v>
+      </c>
+      <c r="K19">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I20" s="70"/>
+      <c r="J20" s="45">
+        <v>130</v>
+      </c>
+      <c r="K20">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21" s="71" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21" s="72"/>
+      <c r="J21" s="45">
+        <v>140</v>
+      </c>
+      <c r="K21">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="H22" s="73" t="s">
+        <v>38</v>
+      </c>
+      <c r="I22" s="74"/>
+      <c r="J22" s="45">
+        <v>139</v>
+      </c>
+      <c r="K22">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="I23" s="76"/>
+      <c r="J23" s="45">
+        <v>135</v>
+      </c>
+      <c r="K23">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="H24" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I24" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="J24" s="45">
+        <v>140</v>
+      </c>
+      <c r="K24">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="G25" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="H25" s="85" t="s">
+        <v>41</v>
+      </c>
+      <c r="I25" s="86"/>
+      <c r="J25" s="45">
+        <v>136</v>
+      </c>
+      <c r="K25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="G26" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="H26" s="83" t="s">
+        <v>42</v>
+      </c>
+      <c r="I26" s="84"/>
+      <c r="J26" s="45">
+        <v>139</v>
+      </c>
+      <c r="K26">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="G27" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="H27" s="81" t="s">
+        <v>43</v>
+      </c>
+      <c r="I27" s="82"/>
+      <c r="J27" s="45">
+        <v>139</v>
+      </c>
+      <c r="K27">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="G28" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="H28" s="79" t="s">
+        <v>44</v>
+      </c>
+      <c r="I28" s="80"/>
+      <c r="J28" s="45">
+        <v>143</v>
+      </c>
+      <c r="K28">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="E29" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="G29" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="H29" s="77" t="s">
+        <v>45</v>
+      </c>
+      <c r="I29" s="78"/>
+      <c r="J29" s="45">
+        <v>141</v>
+      </c>
+      <c r="K29">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="G30" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="H30" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="I30" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="J30" s="45">
+        <v>154</v>
+      </c>
+      <c r="K30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="G31" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="H31" s="67" t="s">
+        <v>40</v>
+      </c>
+      <c r="I31" s="68"/>
+      <c r="J31" s="45">
+        <v>146</v>
+      </c>
+      <c r="K31">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="G32" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="H32" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="I32" s="66"/>
+      <c r="J32" s="45">
+        <v>137</v>
+      </c>
+      <c r="K32">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="F33" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="G33" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="H33" s="63" t="s">
+        <v>48</v>
+      </c>
+      <c r="I33" s="64"/>
+      <c r="J33" s="45">
+        <v>135</v>
+      </c>
+      <c r="K33">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="G34" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="H34" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="I34" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="J34" s="45">
+        <v>134</v>
+      </c>
+      <c r="K34">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H35" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="I35" s="62"/>
+      <c r="J35" s="15">
+        <v>138</v>
+      </c>
+      <c r="K35">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="35">
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="J2:V2"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
     <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:I2"/>
-    <mergeCell ref="H3:I3"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
🎉🎉🎉 Finished Extended-Abstract, finish Master-Thesis. NEXT: revision and submission. 🎉🎉🎉
</commit_message>
<xml_diff>
--- a/Documents/Questoes e Respostas.xlsx
+++ b/Documents/Questoes e Respostas.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PauloGarcia/Desktop/blendingbox/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulogarcia/Desktop/MEIC/blendingbox/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="4300" yWindow="7220" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Perguntas" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="76">
   <si>
     <t>Questão</t>
   </si>
@@ -191,21 +191,6 @@
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>Perguntas com cores dadas iguais:</t>
-  </si>
-  <si>
-    <t>#3 + #12</t>
-  </si>
-  <si>
-    <t>#6 + #11</t>
-  </si>
-  <si>
-    <t>#9 + #15</t>
-  </si>
-  <si>
-    <t>#10 + #13</t>
   </si>
   <si>
     <t>ID</t>
@@ -275,7 +260,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -302,6 +287,12 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -573,7 +564,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -692,161 +683,149 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1153,10 +1132,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M34"/>
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1168,30 +1150,30 @@
     <col min="10" max="10" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:13" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="87" t="s">
+      <c r="C2" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="87"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="87" t="s">
+      <c r="D2" s="59"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="88"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="60"/>
       <c r="J2" s="17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1213,18 +1195,13 @@
       <c r="G3" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="89" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="90"/>
-      <c r="J3" s="7">
-        <v>138</v>
-      </c>
-      <c r="L3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H3" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="62"/>
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1246,21 +1223,13 @@
       <c r="G4" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I4" s="70"/>
-      <c r="J4" s="7">
-        <v>139</v>
-      </c>
-      <c r="L4" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="M4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H4" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="64"/>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1282,21 +1251,13 @@
       <c r="G5" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I5" s="70"/>
-      <c r="J5" s="7">
-        <v>133</v>
-      </c>
-      <c r="L5" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="M5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H5" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="64"/>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1318,21 +1279,13 @@
       <c r="G6" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H6" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I6" s="70"/>
-      <c r="J6" s="7">
-        <v>132</v>
-      </c>
-      <c r="L6" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="M6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H6" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" s="64"/>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1354,21 +1307,13 @@
       <c r="G7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I7" s="70"/>
-      <c r="J7" s="7">
-        <v>138</v>
-      </c>
-      <c r="L7" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="M7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H7" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="64"/>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1390,15 +1335,13 @@
       <c r="G8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I8" s="70"/>
-      <c r="J8" s="7">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H8" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="64"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1420,15 +1363,13 @@
       <c r="G9" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H9" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I9" s="70"/>
-      <c r="J9" s="7">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H9" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="64"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1450,15 +1391,13 @@
       <c r="G10" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H10" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I10" s="70"/>
-      <c r="J10" s="7">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H10" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="64"/>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1480,15 +1419,13 @@
       <c r="G11" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I11" s="70"/>
-      <c r="J11" s="7">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H11" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" s="64"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1510,15 +1447,13 @@
       <c r="G12" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H12" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I12" s="70"/>
-      <c r="J12" s="7">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H12" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="64"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1540,15 +1475,13 @@
       <c r="G13" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H13" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I13" s="70"/>
-      <c r="J13" s="7">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H13" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="64"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1570,15 +1503,13 @@
       <c r="G14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H14" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I14" s="70"/>
-      <c r="J14" s="7">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H14" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14" s="64"/>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -1600,15 +1531,13 @@
       <c r="G15" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H15" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I15" s="70"/>
-      <c r="J15" s="7">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H15" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" s="64"/>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1630,13 +1559,11 @@
       <c r="G16" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H16" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I16" s="70"/>
-      <c r="J16" s="7">
-        <v>133</v>
-      </c>
+      <c r="H16" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" s="64"/>
+      <c r="J16" s="7"/>
     </row>
     <row r="17" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
@@ -1660,13 +1587,11 @@
       <c r="G17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H17" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I17" s="70"/>
-      <c r="J17" s="7">
-        <v>135</v>
-      </c>
+      <c r="H17" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17" s="64"/>
+      <c r="J17" s="7"/>
     </row>
     <row r="18" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
@@ -1690,13 +1615,11 @@
       <c r="G18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H18" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I18" s="70"/>
-      <c r="J18" s="7">
-        <v>140</v>
-      </c>
+      <c r="H18" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I18" s="64"/>
+      <c r="J18" s="7"/>
     </row>
     <row r="19" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
@@ -1720,13 +1643,11 @@
       <c r="G19" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I19" s="70"/>
-      <c r="J19" s="7">
-        <v>130</v>
-      </c>
+      <c r="H19" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19" s="64"/>
+      <c r="J19" s="7"/>
     </row>
     <row r="20" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
@@ -1750,13 +1671,11 @@
       <c r="G20" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H20" s="71" t="s">
+      <c r="H20" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="I20" s="72"/>
-      <c r="J20" s="7">
-        <v>140</v>
-      </c>
+      <c r="I20" s="74"/>
+      <c r="J20" s="7"/>
     </row>
     <row r="21" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
@@ -1780,13 +1699,11 @@
       <c r="G21" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H21" s="73" t="s">
+      <c r="H21" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="I21" s="74"/>
-      <c r="J21" s="7">
-        <v>139</v>
-      </c>
+      <c r="I21" s="76"/>
+      <c r="J21" s="7"/>
     </row>
     <row r="22" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
@@ -1810,13 +1727,11 @@
       <c r="G22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H22" s="75" t="s">
+      <c r="H22" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="I22" s="76"/>
-      <c r="J22" s="7">
-        <v>135</v>
-      </c>
+      <c r="I22" s="78"/>
+      <c r="J22" s="7"/>
     </row>
     <row r="23" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
@@ -1846,9 +1761,7 @@
       <c r="I23" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="J23" s="7">
-        <v>140</v>
-      </c>
+      <c r="J23" s="7"/>
     </row>
     <row r="24" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
@@ -1872,13 +1785,11 @@
       <c r="G24" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H24" s="85" t="s">
+      <c r="H24" s="87" t="s">
         <v>41</v>
       </c>
-      <c r="I24" s="86"/>
-      <c r="J24" s="7">
-        <v>136</v>
-      </c>
+      <c r="I24" s="88"/>
+      <c r="J24" s="7"/>
     </row>
     <row r="25" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
@@ -1902,13 +1813,11 @@
       <c r="G25" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H25" s="83" t="s">
+      <c r="H25" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="I25" s="84"/>
-      <c r="J25" s="7">
-        <v>139</v>
-      </c>
+      <c r="I25" s="86"/>
+      <c r="J25" s="7"/>
     </row>
     <row r="26" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
@@ -1932,13 +1841,11 @@
       <c r="G26" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H26" s="81" t="s">
+      <c r="H26" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="I26" s="82"/>
-      <c r="J26" s="7">
-        <v>139</v>
-      </c>
+      <c r="I26" s="84"/>
+      <c r="J26" s="7"/>
     </row>
     <row r="27" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
@@ -1962,13 +1869,11 @@
       <c r="G27" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H27" s="79" t="s">
+      <c r="H27" s="81" t="s">
         <v>44</v>
       </c>
-      <c r="I27" s="80"/>
-      <c r="J27" s="7">
-        <v>143</v>
-      </c>
+      <c r="I27" s="82"/>
+      <c r="J27" s="7"/>
     </row>
     <row r="28" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
@@ -1992,13 +1897,11 @@
       <c r="G28" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H28" s="77" t="s">
+      <c r="H28" s="79" t="s">
         <v>45</v>
       </c>
-      <c r="I28" s="78"/>
-      <c r="J28" s="7">
-        <v>141</v>
-      </c>
+      <c r="I28" s="80"/>
+      <c r="J28" s="7"/>
     </row>
     <row r="29" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
@@ -2028,9 +1931,7 @@
       <c r="I29" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="J29" s="7">
-        <v>154</v>
-      </c>
+      <c r="J29" s="7"/>
     </row>
     <row r="30" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
@@ -2054,13 +1955,11 @@
       <c r="G30" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H30" s="67" t="s">
+      <c r="H30" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="I30" s="68"/>
-      <c r="J30" s="7">
-        <v>146</v>
-      </c>
+      <c r="I30" s="72"/>
+      <c r="J30" s="7"/>
     </row>
     <row r="31" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
@@ -2084,13 +1983,11 @@
       <c r="G31" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H31" s="65" t="s">
+      <c r="H31" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="I31" s="66"/>
-      <c r="J31" s="7">
-        <v>137</v>
-      </c>
+      <c r="I31" s="70"/>
+      <c r="J31" s="7"/>
     </row>
     <row r="32" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
@@ -2114,13 +2011,11 @@
       <c r="G32" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H32" s="63" t="s">
+      <c r="H32" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="I32" s="64"/>
-      <c r="J32" s="7">
-        <v>135</v>
-      </c>
+      <c r="I32" s="68"/>
+      <c r="J32" s="7"/>
     </row>
     <row r="33" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
@@ -2150,9 +2045,7 @@
       <c r="I33" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="J33" s="7">
-        <v>134</v>
-      </c>
+      <c r="J33" s="7"/>
     </row>
     <row r="34" spans="1:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
@@ -2176,33 +2069,14 @@
       <c r="G34" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="H34" s="61" t="s">
+      <c r="H34" s="65" t="s">
         <v>50</v>
       </c>
-      <c r="I34" s="62"/>
-      <c r="J34" s="15">
-        <v>138</v>
-      </c>
+      <c r="I34" s="66"/>
+      <c r="J34" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
     <mergeCell ref="H34:I34"/>
     <mergeCell ref="H32:I32"/>
     <mergeCell ref="H31:I31"/>
@@ -2217,8 +2091,27 @@
     <mergeCell ref="H26:I26"/>
     <mergeCell ref="H25:I25"/>
     <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="68" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2226,8 +2119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V35"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:K35"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2245,99 +2138,99 @@
   <sheetData>
     <row r="1" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:22" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="89" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="89" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="59"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="91" t="s">
+        <v>75</v>
+      </c>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="63"/>
+      <c r="V2" s="63"/>
+    </row>
+    <row r="3" spans="1:22" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="90"/>
+      <c r="B3" s="90"/>
+      <c r="C3" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="93" t="s">
+      <c r="E3" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="87" t="s">
+      <c r="F3" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="I3" s="60"/>
+      <c r="J3" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="87"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="87" t="s">
+      <c r="K3" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="95" t="s">
-        <v>80</v>
-      </c>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="69"/>
-      <c r="P2" s="69"/>
-      <c r="Q2" s="69"/>
-      <c r="R2" s="69"/>
-      <c r="S2" s="69"/>
-      <c r="T2" s="69"/>
-      <c r="U2" s="69"/>
-      <c r="V2" s="69"/>
-    </row>
-    <row r="3" spans="1:22" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="94"/>
-      <c r="B3" s="94"/>
-      <c r="C3" s="44" t="s">
+      <c r="L3" s="58" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="M3" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="N3" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="G3" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="H3" s="87" t="s">
-        <v>66</v>
-      </c>
-      <c r="I3" s="88"/>
-      <c r="J3" s="45" t="s">
+      <c r="O3" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="K3" s="92" t="s">
+      <c r="P3" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="L3" s="92" t="s">
+      <c r="Q3" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="M3" s="92" t="s">
+      <c r="R3" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="N3" s="92" t="s">
+      <c r="S3" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="O3" s="92" t="s">
+      <c r="T3" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="P3" s="92" t="s">
+      <c r="U3" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="Q3" s="92" t="s">
+      <c r="V3" s="58" t="s">
         <v>74</v>
-      </c>
-      <c r="R3" s="92" t="s">
-        <v>75</v>
-      </c>
-      <c r="S3" s="92" t="s">
-        <v>76</v>
-      </c>
-      <c r="T3" s="92" t="s">
-        <v>77</v>
-      </c>
-      <c r="U3" s="92" t="s">
-        <v>78</v>
-      </c>
-      <c r="V3" s="92" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -2347,33 +2240,33 @@
       <c r="B4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="50" t="s">
+      <c r="C4" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="55" t="s">
+      <c r="F4" s="51" t="s">
         <v>44</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="H4" s="89" t="s">
-        <v>54</v>
-      </c>
-      <c r="I4" s="90"/>
-      <c r="J4" s="45">
+      <c r="H4" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="62"/>
+      <c r="J4" s="41">
         <v>138</v>
       </c>
       <c r="K4">
         <v>29</v>
       </c>
-      <c r="L4" s="91"/>
-      <c r="M4" s="91"/>
+      <c r="L4" s="57"/>
+      <c r="M4" s="57"/>
     </row>
     <row r="5" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -2382,33 +2275,33 @@
       <c r="B5" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="52" t="s">
+      <c r="C5" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="55" t="s">
+      <c r="F5" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="57" t="s">
+      <c r="G5" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I5" s="70"/>
-      <c r="J5" s="45">
+      <c r="H5" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="64"/>
+      <c r="J5" s="41">
         <v>139</v>
       </c>
       <c r="K5">
         <v>29</v>
       </c>
-      <c r="L5" s="92"/>
-      <c r="M5" s="91"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="57"/>
     </row>
     <row r="6" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -2417,33 +2310,33 @@
       <c r="B6" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" s="48" t="s">
+      <c r="C6" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="55" t="s">
+      <c r="F6" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="53" t="s">
+      <c r="G6" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="H6" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I6" s="70"/>
-      <c r="J6" s="45">
+      <c r="H6" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" s="64"/>
+      <c r="J6" s="41">
         <v>133</v>
       </c>
       <c r="K6">
         <v>29</v>
       </c>
-      <c r="L6" s="92"/>
-      <c r="M6" s="91"/>
+      <c r="L6" s="58"/>
+      <c r="M6" s="57"/>
     </row>
     <row r="7" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -2452,33 +2345,33 @@
       <c r="B7" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="44" t="s">
+      <c r="C7" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="40" t="s">
         <v>53</v>
       </c>
       <c r="E7" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="55" t="s">
+      <c r="F7" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="53" t="s">
+      <c r="G7" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I7" s="70"/>
-      <c r="J7" s="45">
+      <c r="H7" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="64"/>
+      <c r="J7" s="41">
         <v>132</v>
       </c>
       <c r="K7">
         <v>29</v>
       </c>
-      <c r="L7" s="92"/>
-      <c r="M7" s="91"/>
+      <c r="L7" s="58"/>
+      <c r="M7" s="57"/>
     </row>
     <row r="8" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
@@ -2487,33 +2380,33 @@
       <c r="B8" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="60" t="s">
+      <c r="C8" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="55" t="s">
+      <c r="F8" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="51" t="s">
+      <c r="G8" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I8" s="70"/>
-      <c r="J8" s="45">
+      <c r="H8" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="64"/>
+      <c r="J8" s="41">
         <v>138</v>
       </c>
       <c r="K8">
         <v>29</v>
       </c>
-      <c r="L8" s="92"/>
-      <c r="M8" s="91"/>
+      <c r="L8" s="58"/>
+      <c r="M8" s="57"/>
     </row>
     <row r="9" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
@@ -2522,33 +2415,33 @@
       <c r="B9" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="59" t="s">
+      <c r="C9" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="55" t="s">
+      <c r="F9" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="49" t="s">
+      <c r="G9" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="H9" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I9" s="70"/>
-      <c r="J9" s="45">
+      <c r="H9" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="64"/>
+      <c r="J9" s="41">
         <v>128</v>
       </c>
       <c r="K9">
         <v>29</v>
       </c>
-      <c r="L9" s="91"/>
-      <c r="M9" s="91"/>
+      <c r="L9" s="57"/>
+      <c r="M9" s="57"/>
     </row>
     <row r="10" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -2557,26 +2450,26 @@
       <c r="B10" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="58" t="s">
+      <c r="C10" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="53" t="s">
+      <c r="F10" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="51" t="s">
+      <c r="G10" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="H10" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I10" s="70"/>
-      <c r="J10" s="45">
+      <c r="H10" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="64"/>
+      <c r="J10" s="41">
         <v>140</v>
       </c>
       <c r="K10">
@@ -2590,26 +2483,26 @@
       <c r="B11" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="56" t="s">
+      <c r="C11" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="51" t="s">
+      <c r="F11" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="49" t="s">
+      <c r="G11" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I11" s="70"/>
-      <c r="J11" s="45">
+      <c r="H11" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" s="64"/>
+      <c r="J11" s="41">
         <v>129</v>
       </c>
       <c r="K11">
@@ -2623,26 +2516,26 @@
       <c r="B12" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="54" t="s">
+      <c r="C12" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="50" t="s">
         <v>45</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G12" s="53" t="s">
+      <c r="G12" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="H12" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I12" s="70"/>
-      <c r="J12" s="45">
+      <c r="H12" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="64"/>
+      <c r="J12" s="41">
         <v>136</v>
       </c>
       <c r="K12">
@@ -2656,26 +2549,26 @@
       <c r="B13" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="47" t="s">
+      <c r="C13" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="43" t="s">
         <v>46</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G13" s="51" t="s">
+      <c r="G13" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="H13" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I13" s="70"/>
-      <c r="J13" s="45">
+      <c r="H13" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="64"/>
+      <c r="J13" s="41">
         <v>136</v>
       </c>
       <c r="K13">
@@ -2689,26 +2582,26 @@
       <c r="B14" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="59" t="s">
+      <c r="C14" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="55" t="s">
         <v>42</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G14" s="51" t="s">
+      <c r="G14" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I14" s="70"/>
-      <c r="J14" s="45">
+      <c r="H14" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14" s="64"/>
+      <c r="J14" s="41">
         <v>130</v>
       </c>
       <c r="K14">
@@ -2722,26 +2615,26 @@
       <c r="B15" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="48" t="s">
+      <c r="C15" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="44" t="s">
         <v>40</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="49" t="s">
+      <c r="G15" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I15" s="70"/>
-      <c r="J15" s="45">
+      <c r="H15" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" s="64"/>
+      <c r="J15" s="41">
         <v>122</v>
       </c>
       <c r="K15">
@@ -2755,26 +2648,26 @@
       <c r="B16" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="47" t="s">
+      <c r="C16" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="57" t="s">
+      <c r="F16" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="G16" s="53" t="s">
+      <c r="G16" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="H16" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I16" s="70"/>
-      <c r="J16" s="45">
+      <c r="H16" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" s="64"/>
+      <c r="J16" s="41">
         <v>135</v>
       </c>
       <c r="K16">
@@ -2788,26 +2681,26 @@
       <c r="B17" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="46" t="s">
+      <c r="C17" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="F17" s="57" t="s">
+      <c r="F17" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="G17" s="51" t="s">
+      <c r="G17" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I17" s="70"/>
-      <c r="J17" s="45">
+      <c r="H17" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17" s="64"/>
+      <c r="J17" s="41">
         <v>133</v>
       </c>
       <c r="K17">
@@ -2821,26 +2714,26 @@
       <c r="B18" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="54" t="s">
+      <c r="C18" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="57" t="s">
+      <c r="F18" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="G18" s="49" t="s">
+      <c r="G18" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="H18" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I18" s="70"/>
-      <c r="J18" s="45">
+      <c r="H18" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I18" s="64"/>
+      <c r="J18" s="41">
         <v>135</v>
       </c>
       <c r="K18">
@@ -2854,26 +2747,26 @@
       <c r="B19" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="44" t="s">
+      <c r="C19" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="40" t="s">
         <v>53</v>
       </c>
       <c r="E19" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="57" t="s">
+      <c r="F19" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="G19" s="49" t="s">
+      <c r="G19" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I19" s="70"/>
-      <c r="J19" s="45">
+      <c r="H19" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19" s="64"/>
+      <c r="J19" s="41">
         <v>140</v>
       </c>
       <c r="K19">
@@ -2887,26 +2780,26 @@
       <c r="B20" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="44" t="s">
+      <c r="C20" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="40" t="s">
         <v>53</v>
       </c>
       <c r="E20" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="53" t="s">
+      <c r="F20" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="49" t="s">
+      <c r="G20" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="H20" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I20" s="70"/>
-      <c r="J20" s="45">
+      <c r="H20" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="I20" s="64"/>
+      <c r="J20" s="41">
         <v>130</v>
       </c>
       <c r="K20">
@@ -2920,26 +2813,26 @@
       <c r="B21" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="55" t="s">
+      <c r="C21" s="51" t="s">
         <v>44</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="G21" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="H21" s="71" t="s">
+      <c r="E21" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="I21" s="72"/>
-      <c r="J21" s="45">
+      <c r="I21" s="74"/>
+      <c r="J21" s="41">
         <v>140</v>
       </c>
       <c r="K21">
@@ -2953,26 +2846,26 @@
       <c r="B22" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="55" t="s">
+      <c r="C22" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="57" t="s">
+      <c r="D22" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="G22" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="H22" s="73" t="s">
+      <c r="E22" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="H22" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="I22" s="74"/>
-      <c r="J22" s="45">
+      <c r="I22" s="76"/>
+      <c r="J22" s="41">
         <v>139</v>
       </c>
       <c r="K22">
@@ -2989,23 +2882,23 @@
       <c r="C23" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="57" t="s">
+      <c r="D23" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="G23" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="H23" s="75" t="s">
+      <c r="E23" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="I23" s="76"/>
-      <c r="J23" s="45">
+      <c r="I23" s="78"/>
+      <c r="J23" s="41">
         <v>135</v>
       </c>
       <c r="K23">
@@ -3019,19 +2912,19 @@
       <c r="B24" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="55" t="s">
+      <c r="C24" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="53" t="s">
+      <c r="D24" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="G24" s="44" t="s">
+      <c r="E24" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" s="40" t="s">
         <v>54</v>
       </c>
       <c r="H24" s="34" t="s">
@@ -3040,7 +2933,7 @@
       <c r="I24" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="J24" s="45">
+      <c r="J24" s="41">
         <v>140</v>
       </c>
       <c r="K24">
@@ -3054,26 +2947,26 @@
       <c r="B25" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="55" t="s">
+      <c r="C25" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="51" t="s">
+      <c r="D25" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="G25" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="H25" s="85" t="s">
+      <c r="E25" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="G25" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="H25" s="87" t="s">
         <v>41</v>
       </c>
-      <c r="I25" s="86"/>
-      <c r="J25" s="45">
+      <c r="I25" s="88"/>
+      <c r="J25" s="41">
         <v>136</v>
       </c>
       <c r="K25">
@@ -3087,26 +2980,26 @@
       <c r="B26" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="55" t="s">
+      <c r="C26" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="49" t="s">
+      <c r="D26" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="G26" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="H26" s="83" t="s">
+      <c r="E26" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="G26" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="H26" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="I26" s="84"/>
-      <c r="J26" s="45">
+      <c r="I26" s="86"/>
+      <c r="J26" s="41">
         <v>139</v>
       </c>
       <c r="K26">
@@ -3120,26 +3013,26 @@
       <c r="B27" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="53" t="s">
+      <c r="C27" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="51" t="s">
+      <c r="D27" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="G27" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="H27" s="81" t="s">
+      <c r="E27" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="G27" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="H27" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="I27" s="82"/>
-      <c r="J27" s="45">
+      <c r="I27" s="84"/>
+      <c r="J27" s="41">
         <v>139</v>
       </c>
       <c r="K27">
@@ -3153,26 +3046,26 @@
       <c r="B28" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="51" t="s">
+      <c r="C28" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="49" t="s">
+      <c r="D28" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="E28" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="F28" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="G28" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="H28" s="79" t="s">
+      <c r="E28" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="G28" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="H28" s="81" t="s">
         <v>44</v>
       </c>
-      <c r="I28" s="80"/>
-      <c r="J28" s="45">
+      <c r="I28" s="82"/>
+      <c r="J28" s="41">
         <v>143</v>
       </c>
       <c r="K28">
@@ -3189,23 +3082,23 @@
       <c r="C29" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="53" t="s">
+      <c r="D29" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="E29" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="G29" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="H29" s="77" t="s">
+      <c r="E29" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="G29" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="H29" s="79" t="s">
         <v>45</v>
       </c>
-      <c r="I29" s="78"/>
-      <c r="J29" s="45">
+      <c r="I29" s="80"/>
+      <c r="J29" s="41">
         <v>141</v>
       </c>
       <c r="K29">
@@ -3222,16 +3115,16 @@
       <c r="C30" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D30" s="51" t="s">
+      <c r="D30" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="E30" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="F30" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="G30" s="44" t="s">
+      <c r="E30" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="G30" s="40" t="s">
         <v>54</v>
       </c>
       <c r="H30" s="36" t="s">
@@ -3240,7 +3133,7 @@
       <c r="I30" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="J30" s="45">
+      <c r="J30" s="41">
         <v>154</v>
       </c>
       <c r="K30">
@@ -3257,23 +3150,23 @@
       <c r="C31" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D31" s="49" t="s">
+      <c r="D31" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="E31" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="F31" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="G31" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="H31" s="67" t="s">
+      <c r="E31" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="G31" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="H31" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="I31" s="68"/>
-      <c r="J31" s="45">
+      <c r="I31" s="72"/>
+      <c r="J31" s="41">
         <v>146</v>
       </c>
       <c r="K31">
@@ -3287,26 +3180,26 @@
       <c r="B32" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C32" s="57" t="s">
+      <c r="C32" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="53" t="s">
+      <c r="D32" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="E32" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="F32" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="G32" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="H32" s="65" t="s">
+      <c r="E32" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="G32" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="H32" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="I32" s="66"/>
-      <c r="J32" s="45">
+      <c r="I32" s="70"/>
+      <c r="J32" s="41">
         <v>137</v>
       </c>
       <c r="K32">
@@ -3320,26 +3213,26 @@
       <c r="B33" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="57" t="s">
+      <c r="C33" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="D33" s="51" t="s">
+      <c r="D33" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="E33" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="F33" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="G33" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="H33" s="63" t="s">
+      <c r="E33" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F33" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="G33" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="H33" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="I33" s="64"/>
-      <c r="J33" s="45">
+      <c r="I33" s="68"/>
+      <c r="J33" s="41">
         <v>135</v>
       </c>
       <c r="K33">
@@ -3353,19 +3246,19 @@
       <c r="B34" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="57" t="s">
+      <c r="C34" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="D34" s="49" t="s">
+      <c r="D34" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="E34" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="F34" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="G34" s="44" t="s">
+      <c r="E34" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="G34" s="40" t="s">
         <v>54</v>
       </c>
       <c r="H34" s="38" t="s">
@@ -3374,7 +3267,7 @@
       <c r="I34" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="J34" s="45">
+      <c r="J34" s="41">
         <v>134</v>
       </c>
       <c r="K34">
@@ -3403,10 +3296,10 @@
       <c r="G35" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="H35" s="61" t="s">
+      <c r="H35" s="65" t="s">
         <v>50</v>
       </c>
-      <c r="I35" s="62"/>
+      <c r="I35" s="66"/>
       <c r="J35" s="15">
         <v>138</v>
       </c>
@@ -3416,6 +3309,25 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
     <mergeCell ref="H35:I35"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="A2:A3"/>
@@ -3432,25 +3344,6 @@
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="H23:I23"/>
     <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>